<commit_message>
Version 1.3.30 (Ch. 0 - Form 2)
</commit_message>
<xml_diff>
--- a/chapters (excel)/SE - Chapter 0 Input.xlsx
+++ b/chapters (excel)/SE - Chapter 0 Input.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="228">
   <si>
     <t>//story[0] === Story Text</t>
   </si>
@@ -225,9 +225,6 @@
   </si>
   <si>
     <t>Of course, I understand.</t>
-  </si>
-  <si>
-    <t>************Not actually a form but rather a page where the player can choose the gender, skin color, hairstyle, etc. of the Scholar************</t>
   </si>
   <si>
     <t>Alright!</t>
@@ -701,13 +698,16 @@
     <t>COPY - PASTE</t>
   </si>
   <si>
-    <t>Hehe, sorry. I didn’t mean to startle you. You must be " + user.username + ".</t>
-  </si>
-  <si>
     <t>C</t>
   </si>
   <si>
     <t>Department Form</t>
+  </si>
+  <si>
+    <t>Hehe, sorry. I didn’t mean to startle you. You must be our new scholar.</t>
+  </si>
+  <si>
+    <t>Choose your name Form</t>
   </si>
 </sst>
 </file>
@@ -1334,7 +1334,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1345,11 +1345,11 @@
   <dimension ref="A1:Z109"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B24" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B27" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A22" sqref="A22"/>
       <selection pane="topRight" activeCell="B22" sqref="B22"/>
       <selection pane="bottomLeft" activeCell="A24" sqref="A24"/>
-      <selection pane="bottomRight" activeCell="B24" sqref="B24"/>
+      <selection pane="bottomRight" activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -1383,7 +1383,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -1404,7 +1404,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>1</v>
@@ -1425,7 +1425,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>2</v>
@@ -1446,7 +1446,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>3</v>
@@ -1467,7 +1467,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>4</v>
@@ -1488,7 +1488,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>5</v>
@@ -1509,7 +1509,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>6</v>
@@ -1530,7 +1530,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>18</v>
@@ -1551,7 +1551,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>34</v>
@@ -1572,7 +1572,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>35</v>
@@ -1593,7 +1593,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>36</v>
@@ -1614,7 +1614,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>39</v>
@@ -1632,7 +1632,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>40</v>
@@ -1647,7 +1647,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>41</v>
@@ -1662,7 +1662,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>42</v>
@@ -1677,7 +1677,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>43</v>
@@ -1692,7 +1692,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>44</v>
@@ -1707,7 +1707,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>45</v>
@@ -1719,7 +1719,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>46</v>
@@ -1731,7 +1731,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>47</v>
@@ -1752,7 +1752,7 @@
         <v>Character 1</v>
       </c>
       <c r="E22" s="13" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F22" s="13" t="str">
         <f t="shared" si="1"/>
@@ -1763,7 +1763,7 @@
         <v>Character 2</v>
       </c>
       <c r="H22" s="13" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I22" s="13" t="str">
         <f t="shared" si="1"/>
@@ -1826,18 +1826,18 @@
         <v>Landing Slide</v>
       </c>
       <c r="X22" s="13" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="Y22" s="13" t="s">
+        <v>199</v>
+      </c>
+      <c r="Z22" s="13" t="s">
         <v>200</v>
-      </c>
-      <c r="Z22" s="13" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A23" s="12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B23" s="13">
         <f>0</f>
@@ -1852,7 +1852,7 @@
         <v>2</v>
       </c>
       <c r="E23" s="13" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F23" s="13">
         <f>1+D23</f>
@@ -1863,7 +1863,7 @@
         <v>4</v>
       </c>
       <c r="H23" s="13" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="I23" s="13">
         <f>1+G23</f>
@@ -1944,7 +1944,7 @@
       <c r="G24" s="7"/>
       <c r="H24" s="7"/>
       <c r="I24" s="8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="J24" s="8"/>
       <c r="K24" s="8"/>
@@ -1980,7 +1980,7 @@
       <c r="G25" s="7"/>
       <c r="H25" s="7"/>
       <c r="I25" s="8" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="J25" s="8"/>
       <c r="K25" s="8"/>
@@ -2016,7 +2016,7 @@
       <c r="G26" s="7"/>
       <c r="H26" s="7"/>
       <c r="I26" s="8" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="J26" s="8"/>
       <c r="K26" s="8"/>
@@ -2050,7 +2050,7 @@
       <c r="G27" s="7"/>
       <c r="H27" s="7"/>
       <c r="I27" s="8" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="J27" s="8"/>
       <c r="K27" s="8"/>
@@ -2084,7 +2084,7 @@
       <c r="G28" s="7"/>
       <c r="H28" s="7"/>
       <c r="I28" s="8" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="J28" s="8"/>
       <c r="K28" s="8"/>
@@ -2103,13 +2103,13 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:26" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A29" s="12">
         <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C29" s="1"/>
       <c r="D29" s="8"/>
@@ -2118,7 +2118,7 @@
       <c r="G29" s="7"/>
       <c r="H29" s="7"/>
       <c r="I29" s="8" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="J29" s="8"/>
       <c r="K29" s="8"/>
@@ -2152,7 +2152,7 @@
       <c r="G30" s="7"/>
       <c r="H30" s="7"/>
       <c r="I30" s="8" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="J30" s="8"/>
       <c r="K30" s="8"/>
@@ -2186,7 +2186,7 @@
       <c r="G31" s="7"/>
       <c r="H31" s="7"/>
       <c r="I31" s="8" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="J31" s="8"/>
       <c r="K31" s="8"/>
@@ -2220,7 +2220,7 @@
       <c r="G32" s="7"/>
       <c r="H32" s="7"/>
       <c r="I32" s="8" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="J32" s="8"/>
       <c r="K32" s="8"/>
@@ -2239,7 +2239,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:26" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A33" s="12">
         <f t="shared" si="5"/>
         <v>9</v>
@@ -2254,7 +2254,7 @@
       <c r="G33" s="7"/>
       <c r="H33" s="7"/>
       <c r="I33" s="8" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="J33" s="8"/>
       <c r="K33" s="8"/>
@@ -2279,7 +2279,7 @@
         <v>10</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C34" s="1"/>
       <c r="D34" s="8"/>
@@ -2288,7 +2288,7 @@
       <c r="G34" s="7"/>
       <c r="H34" s="7"/>
       <c r="I34" s="8" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="J34" s="8"/>
       <c r="K34" s="8"/>
@@ -2307,7 +2307,7 @@
         <v xml:space="preserve">//10 </v>
       </c>
     </row>
-    <row r="35" spans="1:26" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A35" s="12">
         <f t="shared" si="5"/>
         <v>11</v>
@@ -2322,7 +2322,7 @@
       <c r="G35" s="7"/>
       <c r="H35" s="7"/>
       <c r="I35" s="8" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="J35" s="8"/>
       <c r="K35" s="8"/>
@@ -2356,7 +2356,7 @@
       <c r="G36" s="7"/>
       <c r="H36" s="7"/>
       <c r="I36" s="8" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="J36" s="8"/>
       <c r="K36" s="8"/>
@@ -2390,7 +2390,7 @@
       <c r="G37" s="7"/>
       <c r="H37" s="7"/>
       <c r="I37" s="8" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="J37" s="8"/>
       <c r="K37" s="8"/>
@@ -2418,19 +2418,19 @@
         <v>60</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E38" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F38" s="1"/>
       <c r="G38" s="7"/>
       <c r="H38" s="7"/>
       <c r="I38" s="8" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="J38" s="8"/>
       <c r="K38" s="8"/>
@@ -2455,20 +2455,20 @@
         <v>15</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C39" s="1"/>
       <c r="D39" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E39" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F39" s="1"/>
       <c r="G39" s="7"/>
       <c r="H39" s="7"/>
       <c r="I39" s="8" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="J39" s="8"/>
       <c r="K39" s="8"/>
@@ -2487,7 +2487,7 @@
         <v xml:space="preserve">//15 </v>
       </c>
     </row>
-    <row r="40" spans="1:26" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A40" s="12">
         <f t="shared" si="5"/>
         <v>16</v>
@@ -2496,19 +2496,19 @@
         <v>61</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E40" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F40" s="1"/>
       <c r="G40" s="7"/>
       <c r="H40" s="7"/>
       <c r="I40" s="8" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="J40" s="8"/>
       <c r="K40" s="8"/>
@@ -2533,22 +2533,22 @@
         <v>17</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E41" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F41" s="1"/>
       <c r="G41" s="7"/>
       <c r="H41" s="7"/>
       <c r="I41" s="8" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="J41" s="8"/>
       <c r="K41" s="8"/>
@@ -2567,7 +2567,7 @@
         <v/>
       </c>
     </row>
-    <row r="42" spans="1:26" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A42" s="12">
         <f t="shared" si="5"/>
         <v>18</v>
@@ -2576,19 +2576,19 @@
         <v>62</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E42" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F42" s="1"/>
       <c r="G42" s="7"/>
       <c r="H42" s="7"/>
       <c r="I42" s="8" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="J42" s="8"/>
       <c r="K42" s="8"/>
@@ -2613,7 +2613,7 @@
         <v>19</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C43" s="1"/>
       <c r="D43" s="8"/>
@@ -2622,7 +2622,7 @@
       <c r="G43" s="7"/>
       <c r="H43" s="7"/>
       <c r="I43" s="8" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="J43" s="8"/>
       <c r="K43" s="8"/>
@@ -2647,7 +2647,7 @@
         <v>20</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C44" s="1"/>
       <c r="D44" s="8"/>
@@ -2656,7 +2656,7 @@
       <c r="G44" s="7"/>
       <c r="H44" s="7"/>
       <c r="I44" s="8" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J44" s="8"/>
       <c r="K44" s="8"/>
@@ -2675,7 +2675,7 @@
         <v xml:space="preserve">//20 </v>
       </c>
     </row>
-    <row r="45" spans="1:26" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A45" s="12">
         <f t="shared" si="5"/>
         <v>21</v>
@@ -2684,19 +2684,19 @@
         <v>61</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E45" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F45" s="1"/>
       <c r="G45" s="7"/>
       <c r="H45" s="7"/>
       <c r="I45" s="8" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J45" s="8"/>
       <c r="K45" s="8"/>
@@ -2724,19 +2724,19 @@
         <v>61</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E46" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F46" s="1"/>
       <c r="G46" s="7"/>
       <c r="H46" s="7"/>
       <c r="I46" s="8" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J46" s="8"/>
       <c r="K46" s="8"/>
@@ -2761,20 +2761,20 @@
         <v>23</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C47" s="1"/>
       <c r="D47" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E47" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F47" s="1"/>
       <c r="G47" s="7"/>
       <c r="H47" s="7"/>
       <c r="I47" s="8" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J47" s="8"/>
       <c r="K47" s="8"/>
@@ -2808,7 +2808,7 @@
       <c r="G48" s="7"/>
       <c r="H48" s="7"/>
       <c r="I48" s="8" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J48" s="8">
         <v>-3</v>
@@ -2835,20 +2835,20 @@
         <v>25</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C49" s="1"/>
       <c r="D49" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E49" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F49" s="1"/>
       <c r="G49" s="7"/>
       <c r="H49" s="7"/>
       <c r="I49" s="8" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J49" s="8"/>
       <c r="K49" s="8"/>
@@ -2859,7 +2859,7 @@
       <c r="V49" s="1"/>
       <c r="W49" s="1"/>
       <c r="X49" s="11" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="Y49" s="2" t="str">
         <f t="shared" si="3"/>
@@ -2879,19 +2879,19 @@
         <v>61</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E50" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F50" s="1"/>
       <c r="G50" s="7"/>
       <c r="H50" s="7"/>
       <c r="I50" s="8" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J50" s="8"/>
       <c r="K50" s="8"/>
@@ -2919,19 +2919,19 @@
         <v>61</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E51" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F51" s="1"/>
       <c r="G51" s="7"/>
       <c r="H51" s="7"/>
       <c r="I51" s="8" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J51" s="8"/>
       <c r="K51" s="8"/>
@@ -2950,7 +2950,7 @@
         <v/>
       </c>
     </row>
-    <row r="52" spans="1:26" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A52" s="12">
         <f t="shared" si="5"/>
         <v>28</v>
@@ -2959,19 +2959,19 @@
         <v>64</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D52" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E52" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F52" s="1"/>
       <c r="G52" s="7"/>
       <c r="H52" s="7"/>
       <c r="I52" s="8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="J52" s="8"/>
       <c r="K52" s="8"/>
@@ -2990,7 +2990,7 @@
         <v/>
       </c>
     </row>
-    <row r="53" spans="1:26" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A53" s="12">
         <f t="shared" si="5"/>
         <v>29</v>
@@ -2999,19 +2999,19 @@
         <v>65</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E53" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F53" s="1"/>
       <c r="G53" s="7"/>
       <c r="H53" s="7"/>
       <c r="I53" s="8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="J53" s="8"/>
       <c r="K53" s="8"/>
@@ -3040,16 +3040,16 @@
       </c>
       <c r="C54" s="1"/>
       <c r="D54" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E54" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F54" s="1"/>
       <c r="G54" s="7"/>
       <c r="H54" s="7"/>
       <c r="I54" s="8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="J54" s="8"/>
       <c r="K54" s="8"/>
@@ -3074,7 +3074,7 @@
         <v>31</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C55" s="1"/>
       <c r="D55" s="8"/>
@@ -3083,9 +3083,11 @@
       <c r="G55" s="7"/>
       <c r="H55" s="7"/>
       <c r="I55" s="8" t="s">
-        <v>196</v>
-      </c>
-      <c r="J55" s="8"/>
+        <v>195</v>
+      </c>
+      <c r="J55" s="8">
+        <v>-31</v>
+      </c>
       <c r="K55" s="8"/>
       <c r="L55" s="8"/>
       <c r="M55" s="10"/>
@@ -3093,13 +3095,16 @@
       <c r="T55" s="3"/>
       <c r="V55" s="1"/>
       <c r="W55" s="1"/>
+      <c r="X55" s="11" t="s">
+        <v>227</v>
+      </c>
       <c r="Y55" s="2" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="Z55" s="2" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>//31 Choose your name Form</v>
       </c>
     </row>
     <row r="56" spans="1:26" ht="10.15" x14ac:dyDescent="0.2">
@@ -3108,22 +3113,22 @@
         <v>32</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D56" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E56" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F56" s="1"/>
       <c r="G56" s="7"/>
       <c r="H56" s="7"/>
       <c r="I56" s="8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="J56" s="8"/>
       <c r="K56" s="8"/>
@@ -3151,19 +3156,19 @@
         <v>61</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D57" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E57" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F57" s="1"/>
       <c r="G57" s="7"/>
       <c r="H57" s="7"/>
       <c r="I57" s="8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="J57" s="8"/>
       <c r="K57" s="8"/>
@@ -3182,28 +3187,28 @@
         <v/>
       </c>
     </row>
-    <row r="58" spans="1:26" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A58" s="12">
         <f t="shared" si="5"/>
         <v>34</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D58" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E58" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F58" s="1"/>
       <c r="G58" s="7"/>
       <c r="H58" s="7"/>
       <c r="I58" s="8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="J58" s="8"/>
       <c r="K58" s="8"/>
@@ -3228,7 +3233,7 @@
         <v>35</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C59" s="1"/>
       <c r="D59" s="8"/>
@@ -3237,7 +3242,7 @@
       <c r="G59" s="7"/>
       <c r="H59" s="7"/>
       <c r="I59" s="8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="J59" s="8">
         <v>-2</v>
@@ -3247,7 +3252,7 @@
       <c r="M59" s="10"/>
       <c r="N59" s="10"/>
       <c r="Q59" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="T59" s="3"/>
       <c r="V59" s="1"/>
@@ -3267,22 +3272,22 @@
         <v>36</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D60" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E60" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F60" s="1"/>
       <c r="G60" s="7"/>
       <c r="H60" s="7"/>
       <c r="I60" s="8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="J60" s="8"/>
       <c r="K60" s="8"/>
@@ -3310,19 +3315,19 @@
         <v>61</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D61" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E61" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F61" s="1"/>
       <c r="G61" s="7"/>
       <c r="H61" s="7"/>
       <c r="I61" s="8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="J61" s="8"/>
       <c r="K61" s="8"/>
@@ -3350,19 +3355,19 @@
         <v>61</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D62" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E62" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F62" s="1"/>
       <c r="G62" s="7"/>
       <c r="H62" s="7"/>
       <c r="I62" s="8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="J62" s="8"/>
       <c r="K62" s="8"/>
@@ -3381,28 +3386,28 @@
         <v/>
       </c>
     </row>
-    <row r="63" spans="1:26" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A63" s="12">
         <f t="shared" si="5"/>
         <v>39</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D63" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E63" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F63" s="1"/>
       <c r="G63" s="7"/>
       <c r="H63" s="7"/>
       <c r="I63" s="8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="J63" s="8"/>
       <c r="K63" s="8"/>
@@ -3421,28 +3426,28 @@
         <v/>
       </c>
     </row>
-    <row r="64" spans="1:26" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A64" s="12">
         <f t="shared" si="5"/>
         <v>40</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D64" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E64" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F64" s="1"/>
       <c r="G64" s="7"/>
       <c r="H64" s="7"/>
       <c r="I64" s="8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="J64" s="8"/>
       <c r="K64" s="8"/>
@@ -3461,28 +3466,28 @@
         <v xml:space="preserve">//40 </v>
       </c>
     </row>
-    <row r="65" spans="1:26" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A65" s="12">
         <f t="shared" si="5"/>
         <v>41</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D65" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E65" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F65" s="1"/>
       <c r="G65" s="7"/>
       <c r="H65" s="7"/>
       <c r="I65" s="8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="J65" s="8"/>
       <c r="K65" s="8"/>
@@ -3501,7 +3506,7 @@
         <v/>
       </c>
     </row>
-    <row r="66" spans="1:26" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A66" s="12">
         <f t="shared" si="5"/>
         <v>42</v>
@@ -3510,19 +3515,19 @@
         <v>61</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D66" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E66" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F66" s="1"/>
       <c r="G66" s="7"/>
       <c r="H66" s="7"/>
       <c r="I66" s="8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="J66" s="8"/>
       <c r="K66" s="8"/>
@@ -3541,7 +3546,7 @@
         <v/>
       </c>
     </row>
-    <row r="67" spans="1:26" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A67" s="12">
         <f t="shared" si="5"/>
         <v>43</v>
@@ -3550,19 +3555,19 @@
         <v>61</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D67" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E67" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F67" s="1"/>
       <c r="G67" s="7"/>
       <c r="H67" s="7"/>
       <c r="I67" s="8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="J67" s="8"/>
       <c r="K67" s="8"/>
@@ -3581,28 +3586,28 @@
         <v/>
       </c>
     </row>
-    <row r="68" spans="1:26" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A68" s="12">
         <f t="shared" si="5"/>
         <v>44</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D68" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E68" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F68" s="1"/>
       <c r="G68" s="7"/>
       <c r="H68" s="7"/>
       <c r="I68" s="8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="J68" s="8"/>
       <c r="K68" s="8"/>
@@ -3627,22 +3632,22 @@
         <v>45</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D69" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E69" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F69" s="1"/>
       <c r="G69" s="7"/>
       <c r="H69" s="7"/>
       <c r="I69" s="8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="J69" s="8"/>
       <c r="K69" s="8"/>
@@ -3670,19 +3675,19 @@
         <v>61</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D70" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E70" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F70" s="1"/>
       <c r="G70" s="7"/>
       <c r="H70" s="7"/>
       <c r="I70" s="8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="J70" s="8"/>
       <c r="K70" s="8"/>
@@ -3710,19 +3715,19 @@
         <v>61</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D71" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E71" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F71" s="1"/>
       <c r="G71" s="7"/>
       <c r="H71" s="7"/>
       <c r="I71" s="8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="J71" s="8"/>
       <c r="K71" s="8"/>
@@ -3741,7 +3746,7 @@
         <v/>
       </c>
     </row>
-    <row r="72" spans="1:26" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A72" s="12">
         <f t="shared" si="5"/>
         <v>48</v>
@@ -3750,19 +3755,19 @@
         <v>61</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D72" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E72" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F72" s="1"/>
       <c r="G72" s="7"/>
       <c r="H72" s="7"/>
       <c r="I72" s="8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="J72" s="8"/>
       <c r="K72" s="8"/>
@@ -3787,22 +3792,22 @@
         <v>49</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D73" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E73" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F73" s="1"/>
       <c r="G73" s="7"/>
       <c r="H73" s="7"/>
       <c r="I73" s="8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="J73" s="8"/>
       <c r="K73" s="8"/>
@@ -3821,28 +3826,28 @@
         <v/>
       </c>
     </row>
-    <row r="74" spans="1:26" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A74" s="12">
         <f t="shared" si="5"/>
         <v>50</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D74" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E74" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F74" s="1"/>
       <c r="G74" s="7"/>
       <c r="H74" s="7"/>
       <c r="I74" s="8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="J74" s="8"/>
       <c r="K74" s="8"/>
@@ -3870,19 +3875,19 @@
         <v>61</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D75" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E75" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F75" s="1"/>
       <c r="G75" s="7"/>
       <c r="H75" s="7"/>
       <c r="I75" s="8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="J75" s="8"/>
       <c r="K75" s="8"/>
@@ -3914,7 +3919,7 @@
       <c r="G76" s="7"/>
       <c r="H76" s="7"/>
       <c r="I76" s="8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="J76" s="8">
         <v>-2</v>
@@ -3926,7 +3931,7 @@
       <c r="M76" s="10"/>
       <c r="N76" s="10"/>
       <c r="Q76" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="T76" s="3"/>
       <c r="V76" s="1"/>
@@ -3949,19 +3954,19 @@
         <v>61</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D77" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E77" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F77" s="1"/>
       <c r="G77" s="7"/>
       <c r="H77" s="7"/>
       <c r="I77" s="8" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="J77" s="8"/>
       <c r="K77" s="8"/>
@@ -3988,16 +3993,16 @@
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
       <c r="D78" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E78" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F78" s="1"/>
       <c r="G78" s="7"/>
       <c r="H78" s="7"/>
       <c r="I78" s="8" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="J78" s="8">
         <v>-4</v>
@@ -4030,16 +4035,16 @@
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
       <c r="D79" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E79" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F79" s="1"/>
       <c r="G79" s="7"/>
       <c r="H79" s="7"/>
       <c r="I79" s="8" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="J79" s="8">
         <v>-5</v>
@@ -4057,13 +4062,13 @@
         <v>58</v>
       </c>
       <c r="Q79" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="R79" s="8" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="S79" s="8" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="T79" s="3"/>
       <c r="V79" s="1"/>
@@ -4077,28 +4082,28 @@
         <v xml:space="preserve">//55 </v>
       </c>
     </row>
-    <row r="80" spans="1:26" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A80" s="12">
         <f t="shared" si="5"/>
         <v>56</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D80" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E80" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F80" s="1"/>
       <c r="G80" s="7"/>
       <c r="H80" s="7"/>
       <c r="I80" s="8" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="J80" s="8">
         <v>64</v>
@@ -4124,28 +4129,28 @@
         <v/>
       </c>
     </row>
-    <row r="81" spans="1:26" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A81" s="12">
         <f t="shared" si="5"/>
         <v>57</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D81" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E81" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F81" s="1"/>
       <c r="G81" s="7"/>
       <c r="H81" s="7"/>
       <c r="I81" s="8" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="J81" s="8">
         <v>64</v>
@@ -4171,28 +4176,28 @@
         <v/>
       </c>
     </row>
-    <row r="82" spans="1:26" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A82" s="12">
         <f t="shared" si="5"/>
         <v>58</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D82" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E82" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F82" s="1"/>
       <c r="G82" s="7"/>
       <c r="H82" s="7"/>
       <c r="I82" s="8" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="J82" s="8">
         <v>64</v>
@@ -4218,7 +4223,7 @@
         <v/>
       </c>
     </row>
-    <row r="83" spans="1:26" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A83" s="12">
         <f t="shared" si="5"/>
         <v>59</v>
@@ -4226,16 +4231,16 @@
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
       <c r="D83" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E83" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F83" s="1"/>
       <c r="G83" s="7"/>
       <c r="H83" s="7"/>
       <c r="I83" s="8" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="J83" s="8">
         <v>-5</v>
@@ -4253,13 +4258,13 @@
         <v>62</v>
       </c>
       <c r="Q83" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="R83" s="8" t="s">
         <v>206</v>
       </c>
-      <c r="R83" s="8" t="s">
-        <v>207</v>
-      </c>
       <c r="S83" s="8" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="T83" s="3"/>
       <c r="V83" s="1"/>
@@ -4273,28 +4278,28 @@
         <v/>
       </c>
     </row>
-    <row r="84" spans="1:26" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A84" s="12">
         <f t="shared" si="5"/>
         <v>60</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D84" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E84" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F84" s="1"/>
       <c r="G84" s="7"/>
       <c r="H84" s="7"/>
       <c r="I84" s="8" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="J84" s="8">
         <v>64</v>
@@ -4320,28 +4325,28 @@
         <v xml:space="preserve">//60 </v>
       </c>
     </row>
-    <row r="85" spans="1:26" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A85" s="12">
         <f t="shared" si="5"/>
         <v>61</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D85" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E85" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F85" s="1"/>
       <c r="G85" s="7"/>
       <c r="H85" s="7"/>
       <c r="I85" s="8" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="J85" s="8">
         <v>64</v>
@@ -4367,28 +4372,28 @@
         <v/>
       </c>
     </row>
-    <row r="86" spans="1:26" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A86" s="12">
         <f t="shared" si="5"/>
         <v>62</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D86" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E86" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F86" s="1"/>
       <c r="G86" s="7"/>
       <c r="H86" s="7"/>
       <c r="I86" s="8" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="J86" s="8">
         <v>64</v>
@@ -4427,7 +4432,7 @@
       <c r="G87" s="7"/>
       <c r="H87" s="7"/>
       <c r="I87" s="8" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="J87" s="8">
         <v>-2</v>
@@ -4441,7 +4446,7 @@
       <c r="O87" s="10"/>
       <c r="P87" s="10"/>
       <c r="Q87" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="R87" s="10"/>
       <c r="S87" s="10"/>
@@ -4490,7 +4495,7 @@
         <v>70</v>
       </c>
       <c r="X88" s="11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="Y88" s="2" t="str">
         <f t="shared" si="3"/>
@@ -4534,7 +4539,7 @@
         <v>71</v>
       </c>
       <c r="X89" s="11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="Y89" s="2" t="str">
         <f t="shared" ref="Y89:Y109" si="6">IF(MOD(A89,5)=0, "//"&amp;A89, "")</f>
@@ -4580,7 +4585,7 @@
         <v>72</v>
       </c>
       <c r="X90" s="11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="Y90" s="2" t="str">
         <f t="shared" si="6"/>
@@ -4624,7 +4629,7 @@
         <v>70</v>
       </c>
       <c r="X91" s="11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="Y91" s="2" t="str">
         <f t="shared" si="6"/>
@@ -4668,7 +4673,7 @@
         <v>71</v>
       </c>
       <c r="X92" s="11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="Y92" s="2" t="str">
         <f t="shared" si="6"/>
@@ -4712,7 +4717,7 @@
         <v>72</v>
       </c>
       <c r="X93" s="11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="Y93" s="2" t="str">
         <f t="shared" si="6"/>
@@ -4723,28 +4728,28 @@
         <v>//69 ghost slide</v>
       </c>
     </row>
-    <row r="94" spans="1:26" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A94" s="12">
         <f t="shared" si="8"/>
         <v>70</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D94" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E94" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F94" s="1"/>
       <c r="G94" s="7"/>
       <c r="H94" s="7"/>
       <c r="I94" s="8" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J94" s="8">
         <v>74</v>
@@ -4770,28 +4775,28 @@
         <v xml:space="preserve">//70 </v>
       </c>
     </row>
-    <row r="95" spans="1:26" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A95" s="12">
         <f t="shared" si="8"/>
         <v>71</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D95" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E95" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F95" s="1"/>
       <c r="G95" s="7"/>
       <c r="H95" s="7"/>
       <c r="I95" s="8" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J95" s="8">
         <v>74</v>
@@ -4823,22 +4828,22 @@
         <v>72</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D96" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E96" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F96" s="1"/>
       <c r="G96" s="7"/>
       <c r="H96" s="7"/>
       <c r="I96" s="8" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J96" s="8">
         <v>74</v>
@@ -4864,32 +4869,32 @@
         <v/>
       </c>
     </row>
-    <row r="97" spans="1:26" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A97" s="12">
         <f t="shared" si="8"/>
         <v>73</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D97" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E97" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F97" s="1"/>
       <c r="G97" s="8" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="H97" s="7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I97" s="8" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J97" s="8"/>
       <c r="K97" s="8"/>
@@ -4913,32 +4918,32 @@
         <v/>
       </c>
     </row>
-    <row r="98" spans="1:26" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A98" s="12">
         <f t="shared" si="8"/>
         <v>74</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D98" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E98" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F98" s="1"/>
       <c r="G98" s="8" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="H98" s="7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I98" s="8" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J98" s="8"/>
       <c r="K98" s="8"/>
@@ -4962,32 +4967,32 @@
         <v/>
       </c>
     </row>
-    <row r="99" spans="1:26" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A99" s="12">
         <f t="shared" si="8"/>
         <v>75</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D99" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E99" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F99" s="1"/>
       <c r="G99" s="8" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="H99" s="7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I99" s="8" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J99" s="8"/>
       <c r="K99" s="8"/>
@@ -5011,30 +5016,30 @@
         <v xml:space="preserve">//75 </v>
       </c>
     </row>
-    <row r="100" spans="1:26" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A100" s="12">
         <f t="shared" si="8"/>
         <v>76</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C100" s="1"/>
       <c r="D100" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E100" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F100" s="1"/>
       <c r="G100" s="8" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="H100" s="7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I100" s="8" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J100" s="8"/>
       <c r="K100" s="8"/>
@@ -5058,30 +5063,30 @@
         <v/>
       </c>
     </row>
-    <row r="101" spans="1:26" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A101" s="12">
         <f t="shared" si="8"/>
         <v>77</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C101" s="1"/>
       <c r="D101" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E101" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F101" s="1"/>
       <c r="G101" s="8" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="H101" s="7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I101" s="8" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J101" s="8"/>
       <c r="K101" s="8"/>
@@ -5105,30 +5110,30 @@
         <v/>
       </c>
     </row>
-    <row r="102" spans="1:26" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A102" s="12">
         <f t="shared" si="8"/>
         <v>78</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C102" s="1"/>
       <c r="D102" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E102" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F102" s="1"/>
       <c r="G102" s="8" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="H102" s="7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I102" s="8" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J102" s="8"/>
       <c r="K102" s="8"/>
@@ -5152,32 +5157,32 @@
         <v/>
       </c>
     </row>
-    <row r="103" spans="1:26" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A103" s="12">
         <f t="shared" si="8"/>
         <v>79</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D103" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E103" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F103" s="1"/>
       <c r="G103" s="8" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="H103" s="7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I103" s="8" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J103" s="8"/>
       <c r="K103" s="8"/>
@@ -5201,32 +5206,32 @@
         <v/>
       </c>
     </row>
-    <row r="104" spans="1:26" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A104" s="12">
         <f t="shared" si="8"/>
         <v>80</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C104" s="1"/>
       <c r="D104" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E104" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="F104" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="G104" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="H104" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="F104" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="G104" s="8" t="s">
-        <v>188</v>
-      </c>
-      <c r="H104" s="7" t="s">
-        <v>172</v>
-      </c>
       <c r="I104" s="8" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J104" s="8"/>
       <c r="K104" s="8"/>
@@ -5250,32 +5255,32 @@
         <v xml:space="preserve">//80 </v>
       </c>
     </row>
-    <row r="105" spans="1:26" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A105" s="12">
         <f t="shared" si="8"/>
         <v>81</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C105" s="1"/>
       <c r="D105" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E105" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="F105" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="G105" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="H105" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="F105" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="G105" s="8" t="s">
-        <v>188</v>
-      </c>
-      <c r="H105" s="7" t="s">
-        <v>172</v>
-      </c>
       <c r="I105" s="8" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J105" s="8"/>
       <c r="K105" s="8"/>
@@ -5299,30 +5304,30 @@
         <v/>
       </c>
     </row>
-    <row r="106" spans="1:26" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A106" s="12">
         <f t="shared" si="8"/>
         <v>82</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C106" s="1"/>
       <c r="D106" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E106" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F106" s="1"/>
       <c r="G106" s="8" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="H106" s="7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I106" s="8" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J106" s="8"/>
       <c r="K106" s="8"/>
@@ -5346,32 +5351,32 @@
         <v/>
       </c>
     </row>
-    <row r="107" spans="1:26" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A107" s="12">
         <f t="shared" si="8"/>
         <v>83</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D107" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E107" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F107" s="1"/>
       <c r="G107" s="8" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="H107" s="7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I107" s="8" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J107" s="8"/>
       <c r="K107" s="8"/>
@@ -5395,28 +5400,28 @@
         <v/>
       </c>
     </row>
-    <row r="108" spans="1:26" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A108" s="12">
         <f t="shared" si="8"/>
         <v>84</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C108" s="1"/>
       <c r="D108" s="8" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E108" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F108" s="1"/>
       <c r="G108" s="8"/>
       <c r="H108" s="7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I108" s="8" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J108" s="8"/>
       <c r="K108" s="8"/>
@@ -5440,30 +5445,30 @@
         <v/>
       </c>
     </row>
-    <row r="109" spans="1:26" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A109" s="12">
         <f t="shared" si="8"/>
         <v>85</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D109" s="8" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E109" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F109" s="1"/>
       <c r="G109" s="8"/>
       <c r="H109" s="7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I109" s="8" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J109" s="8"/>
       <c r="K109" s="8"/>
@@ -5572,23 +5577,23 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="1"/>
       <c r="N1" s="6" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="R1" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:26" ht="10.15" x14ac:dyDescent="0.2">
@@ -5597,20 +5602,20 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="1"/>
       <c r="N2" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="O2" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="O2" s="2" t="s">
-        <v>169</v>
-      </c>
       <c r="Q2" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="R2" s="4">
         <f>0</f>
@@ -5633,20 +5638,20 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D3" s="1"/>
       <c r="N3" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="R3" s="4">
         <f>1+R2</f>
@@ -5669,20 +5674,20 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="1"/>
       <c r="N4" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="R4" s="4">
         <f>1+R3</f>
@@ -5704,20 +5709,20 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D5" s="1"/>
       <c r="N5" s="4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="R5" s="4">
         <f>1+R4</f>
@@ -5739,20 +5744,20 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D6" s="1"/>
       <c r="N6" s="4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="O6" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="R6" s="4">
         <f>1+R5</f>
@@ -5774,20 +5779,20 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D7" s="1"/>
       <c r="N7" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="Q7" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="R7" s="4">
         <f>1+R6</f>
@@ -5809,17 +5814,17 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D8" s="1"/>
       <c r="N8" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="O8" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="V8" s="1" t="s">
         <v>12</v>
@@ -5837,17 +5842,17 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>34</v>
       </c>
       <c r="D9" s="1"/>
       <c r="N9" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="V9" s="1" t="s">
         <v>13</v>
@@ -5865,17 +5870,17 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>35</v>
       </c>
       <c r="D10" s="1"/>
       <c r="N10" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="O10" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="V10" s="1" t="s">
         <v>14</v>
@@ -5893,17 +5898,17 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>36</v>
       </c>
       <c r="D11" s="1"/>
       <c r="N11" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="O11" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="V11" s="1" t="s">
         <v>15</v>
@@ -5921,17 +5926,17 @@
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>39</v>
       </c>
       <c r="D12" s="1"/>
       <c r="N12" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="O12" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="V12" s="1" t="s">
         <v>16</v>
@@ -5949,17 +5954,17 @@
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>40</v>
       </c>
       <c r="D13" s="1"/>
       <c r="N13" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="O13" s="2" t="s">
         <v>188</v>
-      </c>
-      <c r="O13" s="2" t="s">
-        <v>189</v>
       </c>
       <c r="V13" s="1" t="s">
         <v>17</v>
@@ -5974,7 +5979,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>41</v>
@@ -5990,7 +5995,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>42</v>
@@ -6006,7 +6011,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>43</v>
@@ -6022,7 +6027,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>44</v>
@@ -6032,13 +6037,13 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:24" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>45</v>
@@ -6051,7 +6056,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>46</v>
@@ -6064,7 +6069,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>47</v>
@@ -6162,7 +6167,7 @@
         <v>19</v>
       </c>
       <c r="V22" s="27" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="23" spans="1:24" ht="10.15" x14ac:dyDescent="0.2">
@@ -6248,7 +6253,7 @@
         <v>Landing Slide</v>
       </c>
       <c r="V23" s="17" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="24" spans="1:24" ht="10.15" x14ac:dyDescent="0.2">
@@ -6334,12 +6339,12 @@
         <v>//story[19] === landing slide -&gt; -1 by defaut, but we go to a specific slide after the current one</v>
       </c>
       <c r="V24" s="11" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="25" spans="1:24" ht="10.15" x14ac:dyDescent="0.2">
       <c r="A25" s="15" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B25" s="20" t="str">
         <f>"story["&amp;B22&amp;"] = ["</f>
@@ -8955,7 +8960,7 @@
 "];",IF('Chapter 0 (Input)'!C40="",
 """"&amp;"null"&amp;""""&amp;",",
 """"&amp;'Chapter 0 (Input)'!C40&amp;""""&amp;",")&amp;$V42)</f>
-        <v>"Hehe, sorry. I didn’t mean to startle you. You must be " + user.username + ".",</v>
+        <v>"Hehe, sorry. I didn’t mean to startle you. You must be our new scholar.",</v>
       </c>
       <c r="D42" s="5" t="str">
         <f>IF(D43="",
@@ -11303,14 +11308,14 @@
 IF('Chapter 0 (Input)'!B55="",
 """"&amp;"null"&amp;""""&amp;",",
 """"&amp;'Chapter 0 (Input)'!B55&amp;""""&amp;",")&amp;$V57)</f>
-        <v>"************Not actually a form but rather a page where the player can choose the gender, skin color, hairstyle, etc. of the Scholar************",</v>
+        <v>"Click here to submit",//31 Choose your name Form</v>
       </c>
       <c r="C57" s="5" t="str">
         <f>IF(C58="",
 "];",IF('Chapter 0 (Input)'!C55="",
 """"&amp;"null"&amp;""""&amp;",",
 """"&amp;'Chapter 0 (Input)'!C55&amp;""""&amp;",")&amp;$V57)</f>
-        <v>"null",</v>
+        <v>"null",//31 Choose your name Form</v>
       </c>
       <c r="D57" s="5" t="str">
         <f>IF(D58="",
@@ -11321,14 +11326,14 @@
 "[" &amp;
 VLOOKUP('Chapter 0 (Input)'!E55,$Q$2:$R$13,2,FALSE) &amp;
 "],")&amp;$V57)</f>
-        <v>"null",</v>
+        <v>"null",//31 Choose your name Form</v>
       </c>
       <c r="E57" s="5" t="str">
         <f>IF(E58="",
 "];",IF('Chapter 0 (Input)'!F55="",
 """"&amp;"null"&amp;""""&amp;",",
 """"&amp;'Chapter 0 (Input)'!F55&amp;""""&amp;",")&amp;$V57)</f>
-        <v>"null",</v>
+        <v>"null",//31 Choose your name Form</v>
       </c>
       <c r="F57" s="5" t="str">
         <f>IF(F58="",
@@ -11339,7 +11344,7 @@
 "[" &amp;
 VLOOKUP('Chapter 0 (Input)'!H55, $Q$2:$R$13,2,FALSE) &amp;
 "],")&amp;$V57)</f>
-        <v>"null",</v>
+        <v>"null",//31 Choose your name Form</v>
       </c>
       <c r="G57" s="4" t="str">
         <f>IF(G58="",
@@ -11347,106 +11352,106 @@
 """"&amp;"null"&amp;""""&amp;",",
 "locations."&amp;
 'Chapter 0 (Input)'!I55&amp;",")&amp;$V57)</f>
-        <v>locations.dorm,</v>
+        <v>locations.dorm,//31 Choose your name Form</v>
       </c>
       <c r="H57" s="4" t="str">
         <f>IF(H58="",
 "];",IF('Chapter 0 (Input)'!J55="",
 "-1"&amp;",",
 'Chapter 0 (Input)'!J55&amp;",")&amp;$V57)</f>
-        <v>-1,</v>
+        <v>-31,//31 Choose your name Form</v>
       </c>
       <c r="I57" s="4" t="str">
         <f>IF(I58="",
 "];",IF('Chapter 0 (Input)'!K55="",
 "0"&amp;",",
 'Chapter 0 (Input)'!K55&amp;",")&amp;$V57)</f>
-        <v>0,</v>
+        <v>0,//31 Choose your name Form</v>
       </c>
       <c r="J57" s="4" t="str">
         <f>IF(J58="",
 "];",IF('Chapter 0 (Input)'!L55="",
 "-1"&amp;",",
 'Chapter 0 (Input)'!L55&amp;",")&amp;$V57)</f>
-        <v>-1,</v>
+        <v>-1,//31 Choose your name Form</v>
       </c>
       <c r="K57" s="4" t="str">
         <f>IF(K58="",
 "];",IF('Chapter 0 (Input)'!M55="",
 "-1"&amp;",",
 'Chapter 0 (Input)'!M55&amp;",")&amp;$V57)</f>
-        <v>-1,</v>
+        <v>-1,//31 Choose your name Form</v>
       </c>
       <c r="L57" s="4" t="str">
         <f>IF(L58="",
 "];",IF('Chapter 0 (Input)'!N55="",
 "-1"&amp;",",
 'Chapter 0 (Input)'!N55&amp;",")&amp;$V57)</f>
-        <v>-1,</v>
+        <v>-1,//31 Choose your name Form</v>
       </c>
       <c r="M57" s="4" t="str">
         <f>IF(M58="",
 "];",IF('Chapter 0 (Input)'!O55="",
 "-1"&amp;",",
 'Chapter 0 (Input)'!O55&amp;",")&amp;$V57)</f>
-        <v>-1,</v>
+        <v>-1,//31 Choose your name Form</v>
       </c>
       <c r="N57" s="4" t="str">
         <f>IF(N58="",
 "];",IF('Chapter 0 (Input)'!P55="",
 "-1"&amp;",",
 'Chapter 0 (Input)'!P55&amp;",")&amp;$V57)</f>
-        <v>-1,</v>
+        <v>-1,//31 Choose your name Form</v>
       </c>
       <c r="O57" s="4" t="str">
         <f>IF(O58="",
 "];",IF('Chapter 0 (Input)'!Q55="",
 """"&amp;"null"&amp;""""&amp;",",
 """"&amp;'Chapter 0 (Input)'!Q55&amp;""""&amp;",")&amp;$V57)</f>
-        <v>"null",</v>
+        <v>"null",//31 Choose your name Form</v>
       </c>
       <c r="P57" s="4" t="str">
         <f>IF(P58="",
 "];",IF('Chapter 0 (Input)'!R55="",
 """"&amp;"null"&amp;""""&amp;",",
 """"&amp;'Chapter 0 (Input)'!R55&amp;""""&amp;",")&amp;$V57)</f>
-        <v>"null",</v>
+        <v>"null",//31 Choose your name Form</v>
       </c>
       <c r="Q57" s="4" t="str">
         <f>IF(Q58="",
 "];",IF('Chapter 0 (Input)'!S55="",
 """"&amp;"null"&amp;""""&amp;",",
 """"&amp;'Chapter 0 (Input)'!S55&amp;""""&amp;",")&amp;$V57)</f>
-        <v>"null",</v>
+        <v>"null",//31 Choose your name Form</v>
       </c>
       <c r="R57" s="4" t="str">
         <f>IF(R58="",
 "];",IF('Chapter 0 (Input)'!T55="",
 "0"&amp;",",
 'Chapter 0 (Input)'!T55&amp;",")&amp;$V57)</f>
-        <v>0,</v>
+        <v>0,//31 Choose your name Form</v>
       </c>
       <c r="S57" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>false,</v>
+        <v>false,//31 Choose your name Form</v>
       </c>
       <c r="T57" s="4" t="str">
         <f>IF(T58="",
 "];",IF('Chapter 0 (Input)'!V55="",
 "-1"&amp;",",
 'Chapter 0 (Input)'!V55&amp;",")&amp;$V57)</f>
-        <v>-1,</v>
+        <v>-1,//31 Choose your name Form</v>
       </c>
       <c r="U57" s="4" t="str">
         <f>IF(U58="",
 "];",IF('Chapter 0 (Input)'!W55="",
 "-1"&amp;",",
 'Chapter 0 (Input)'!W55&amp;",")&amp;$V57)</f>
-        <v>-1,</v>
+        <v>-1,//31 Choose your name Form</v>
       </c>
       <c r="V57" s="22" t="str">
         <f>'Chapter 0 (Input)'!Z55</f>
-        <v/>
+        <v>//31 Choose your name Form</v>
       </c>
     </row>
     <row r="58" spans="1:22" ht="10.15" x14ac:dyDescent="0.2">
@@ -18516,7 +18521,7 @@
         <v/>
       </c>
     </row>
-    <row r="103" spans="1:22" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A103" s="16">
         <f t="shared" si="7"/>
         <v>77</v>
@@ -18673,7 +18678,7 @@
         <v/>
       </c>
     </row>
-    <row r="104" spans="1:22" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A104" s="16">
         <f t="shared" si="7"/>
         <v>78</v>
@@ -18830,7 +18835,7 @@
         <v/>
       </c>
     </row>
-    <row r="105" spans="1:22" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A105" s="16">
         <f t="shared" si="7"/>
         <v>79</v>
@@ -18987,7 +18992,7 @@
         <v/>
       </c>
     </row>
-    <row r="106" spans="1:22" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A106" s="16">
         <f t="shared" si="7"/>
         <v>80</v>
@@ -19144,7 +19149,7 @@
         <v xml:space="preserve">//80 </v>
       </c>
     </row>
-    <row r="107" spans="1:22" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A107" s="16">
         <f t="shared" si="7"/>
         <v>81</v>
@@ -19301,7 +19306,7 @@
         <v/>
       </c>
     </row>
-    <row r="108" spans="1:22" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A108" s="16">
         <f t="shared" si="7"/>
         <v>82</v>
@@ -19458,7 +19463,7 @@
         <v/>
       </c>
     </row>
-    <row r="109" spans="1:22" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A109" s="16">
         <f t="shared" si="7"/>
         <v>83</v>
@@ -19615,9 +19620,9 @@
         <v/>
       </c>
     </row>
-    <row r="110" spans="1:22" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A110" s="16">
-        <f t="shared" ref="A110:A173" si="9">1+A109</f>
+        <f t="shared" ref="A110:A111" si="9">1+A109</f>
         <v>84</v>
       </c>
       <c r="B110" s="5" t="str">
@@ -19772,7 +19777,7 @@
         <v/>
       </c>
     </row>
-    <row r="111" spans="1:22" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A111" s="16">
         <f t="shared" si="9"/>
         <v>85</v>
@@ -20083,346 +20088,346 @@
       </c>
       <c r="V112" s="22"/>
     </row>
-    <row r="113" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="113" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B113" s="3"/>
     </row>
-    <row r="114" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="114" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B114" s="3"/>
     </row>
-    <row r="115" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="115" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B115" s="3"/>
     </row>
-    <row r="116" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="116" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B116" s="3"/>
     </row>
-    <row r="117" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="117" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B117" s="3"/>
     </row>
-    <row r="118" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="118" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B118" s="3"/>
     </row>
-    <row r="119" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="119" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B119" s="3"/>
     </row>
-    <row r="120" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="120" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B120" s="3"/>
     </row>
-    <row r="121" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="121" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B121" s="3"/>
     </row>
-    <row r="122" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="122" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B122" s="3"/>
     </row>
-    <row r="123" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="123" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B123" s="3"/>
     </row>
-    <row r="124" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="124" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B124" s="3"/>
     </row>
-    <row r="125" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="125" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B125" s="3"/>
     </row>
-    <row r="126" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="126" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B126" s="3"/>
     </row>
-    <row r="127" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="127" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B127" s="3"/>
     </row>
-    <row r="128" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="128" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B128" s="3"/>
     </row>
-    <row r="129" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="129" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B129" s="3"/>
     </row>
-    <row r="130" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="130" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B130" s="3"/>
     </row>
-    <row r="131" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="131" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B131" s="3"/>
     </row>
-    <row r="132" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="132" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B132" s="3"/>
     </row>
-    <row r="133" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="133" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B133" s="3"/>
     </row>
-    <row r="134" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="134" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B134" s="3"/>
     </row>
-    <row r="135" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="135" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B135" s="3"/>
     </row>
-    <row r="136" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="136" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B136" s="3"/>
     </row>
-    <row r="137" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="137" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B137" s="3"/>
     </row>
-    <row r="138" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="138" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B138" s="3"/>
     </row>
-    <row r="139" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="139" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B139" s="3"/>
     </row>
-    <row r="140" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="140" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B140" s="3"/>
     </row>
-    <row r="141" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="141" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B141" s="3"/>
     </row>
-    <row r="142" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="142" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B142" s="3"/>
     </row>
-    <row r="143" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="143" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B143" s="3"/>
     </row>
-    <row r="144" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="144" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B144" s="3"/>
     </row>
-    <row r="145" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="145" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B145" s="3"/>
     </row>
-    <row r="146" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="146" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B146" s="3"/>
     </row>
-    <row r="147" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="147" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B147" s="3"/>
     </row>
-    <row r="148" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="148" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B148" s="3"/>
     </row>
-    <row r="149" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="149" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B149" s="3"/>
     </row>
-    <row r="150" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="150" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B150" s="3"/>
     </row>
-    <row r="151" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="151" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B151" s="3"/>
     </row>
-    <row r="152" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="152" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B152" s="3"/>
     </row>
-    <row r="153" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="153" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B153" s="3"/>
     </row>
-    <row r="154" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="154" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B154" s="3"/>
     </row>
-    <row r="155" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="155" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B155" s="3"/>
     </row>
-    <row r="156" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="156" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B156" s="3"/>
     </row>
-    <row r="157" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="157" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B157" s="3"/>
     </row>
-    <row r="158" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="158" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B158" s="3"/>
     </row>
-    <row r="159" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="159" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B159" s="3"/>
     </row>
-    <row r="160" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="160" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B160" s="3"/>
     </row>
-    <row r="161" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="161" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B161" s="3"/>
     </row>
-    <row r="162" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="162" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B162" s="3"/>
     </row>
-    <row r="163" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="163" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B163" s="3"/>
     </row>
-    <row r="164" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="164" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B164" s="3"/>
     </row>
-    <row r="165" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="165" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B165" s="3"/>
     </row>
-    <row r="166" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="166" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B166" s="3"/>
     </row>
-    <row r="167" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="167" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B167" s="3"/>
     </row>
-    <row r="168" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="168" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B168" s="3"/>
     </row>
-    <row r="169" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="169" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B169" s="3"/>
     </row>
-    <row r="170" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="170" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B170" s="3"/>
     </row>
-    <row r="171" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="171" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B171" s="3"/>
     </row>
-    <row r="172" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="172" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B172" s="3"/>
     </row>
-    <row r="173" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="173" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B173" s="3"/>
     </row>
-    <row r="174" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="174" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B174" s="3"/>
     </row>
-    <row r="175" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="175" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B175" s="3"/>
     </row>
-    <row r="176" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="176" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B176" s="3"/>
     </row>
-    <row r="177" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="177" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B177" s="3"/>
     </row>
-    <row r="178" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="178" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B178" s="3"/>
     </row>
-    <row r="179" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="179" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B179" s="3"/>
     </row>
-    <row r="180" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="180" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B180" s="3"/>
     </row>
-    <row r="181" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="181" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B181" s="3"/>
     </row>
-    <row r="182" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="182" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B182" s="3"/>
     </row>
-    <row r="183" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="183" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B183" s="3"/>
     </row>
-    <row r="184" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="184" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B184" s="3"/>
     </row>
-    <row r="185" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="185" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B185" s="3"/>
     </row>
-    <row r="186" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="186" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B186" s="3"/>
     </row>
-    <row r="187" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="187" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B187" s="3"/>
     </row>
-    <row r="188" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="188" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B188" s="3"/>
     </row>
-    <row r="189" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="189" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B189" s="3"/>
     </row>
-    <row r="190" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="190" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B190" s="3"/>
     </row>
-    <row r="191" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="191" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B191" s="3"/>
     </row>
-    <row r="192" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="192" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B192" s="3"/>
     </row>
-    <row r="193" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="193" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B193" s="3"/>
     </row>
-    <row r="194" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="194" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B194" s="3"/>
     </row>
-    <row r="195" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="195" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B195" s="3"/>
     </row>
-    <row r="196" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="196" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B196" s="3"/>
     </row>
-    <row r="197" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="197" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B197" s="3"/>
     </row>
-    <row r="198" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="198" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B198" s="3"/>
     </row>
-    <row r="199" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="199" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B199" s="3"/>
     </row>
-    <row r="200" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="200" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B200" s="3"/>
     </row>
-    <row r="201" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="201" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B201" s="3"/>
     </row>
-    <row r="202" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="202" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B202" s="3"/>
     </row>
-    <row r="203" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="203" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B203" s="3"/>
     </row>
-    <row r="204" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="204" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B204" s="3"/>
     </row>
-    <row r="205" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="205" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B205" s="3"/>
     </row>
-    <row r="206" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="206" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B206" s="3"/>
     </row>
-    <row r="207" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="207" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B207" s="3"/>
     </row>
-    <row r="208" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="208" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B208" s="3"/>
     </row>
-    <row r="209" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="209" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B209" s="3"/>
     </row>
-    <row r="210" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="210" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B210" s="3"/>
     </row>
-    <row r="211" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="211" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B211" s="3"/>
     </row>
-    <row r="212" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="212" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B212" s="3"/>
     </row>
-    <row r="213" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="213" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B213" s="3"/>
     </row>
-    <row r="214" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="214" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B214" s="3"/>
     </row>
-    <row r="215" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="215" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B215" s="3"/>
     </row>
-    <row r="216" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="216" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B216" s="3"/>
     </row>
-    <row r="217" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="217" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B217" s="3"/>
     </row>
-    <row r="218" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="218" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B218" s="3"/>
     </row>
-    <row r="219" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="219" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B219" s="3"/>
     </row>
-    <row r="220" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="220" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B220" s="3"/>
     </row>
-    <row r="221" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="221" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B221" s="3"/>
     </row>
-    <row r="222" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="222" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B222" s="3"/>
     </row>
-    <row r="223" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="223" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B223" s="3"/>
     </row>
-    <row r="224" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="224" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B224" s="3"/>
     </row>
-    <row r="225" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="225" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B225" s="3"/>
     </row>
-    <row r="226" spans="2:2" ht="10.15" x14ac:dyDescent="0.2">
+    <row r="226" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B226" s="3"/>
     </row>
   </sheetData>
@@ -20459,19 +20464,19 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="24" t="s">
+        <v>218</v>
+      </c>
+      <c r="B1" s="24" t="s">
         <v>219</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="D1" s="24" t="s">
+        <v>221</v>
+      </c>
+      <c r="E1" s="24" t="s">
         <v>220</v>
       </c>
-      <c r="D1" s="24" t="s">
-        <v>222</v>
-      </c>
-      <c r="E1" s="24" t="s">
-        <v>221</v>
-      </c>
       <c r="G1" s="25" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -20955,7 +20960,7 @@
       </c>
       <c r="G35" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>"************Not actually a form but rather a page where the player can choose the gender, skin color, hairstyle, etc. of the Scholar************",</v>
+        <v>"Click here to submit",//31 Choose your name Form</v>
       </c>
     </row>
     <row r="36" spans="4:7" x14ac:dyDescent="0.2">
@@ -21991,7 +21996,7 @@
       </c>
       <c r="G109" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>"Hehe, sorry. I didn’t mean to startle you. You must be " + user.username + ".",</v>
+        <v>"Hehe, sorry. I didn’t mean to startle you. You must be our new scholar.",</v>
       </c>
     </row>
     <row r="110" spans="4:7" x14ac:dyDescent="0.2">
@@ -22201,7 +22206,7 @@
       </c>
       <c r="G124" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>"null",</v>
+        <v>"null",//31 Choose your name Form</v>
       </c>
     </row>
     <row r="125" spans="4:7" x14ac:dyDescent="0.2">
@@ -23447,7 +23452,7 @@
       </c>
       <c r="G213" s="2" t="str">
         <f t="shared" si="7"/>
-        <v>"null",</v>
+        <v>"null",//31 Choose your name Form</v>
       </c>
     </row>
     <row r="214" spans="4:7" x14ac:dyDescent="0.2">
@@ -24693,7 +24698,7 @@
       </c>
       <c r="G302" s="2" t="str">
         <f t="shared" si="9"/>
-        <v>"null",</v>
+        <v>"null",//31 Choose your name Form</v>
       </c>
     </row>
     <row r="303" spans="4:7" x14ac:dyDescent="0.2">
@@ -25939,7 +25944,7 @@
       </c>
       <c r="G391" s="2" t="str">
         <f t="shared" si="13"/>
-        <v>"null",</v>
+        <v>"null",//31 Choose your name Form</v>
       </c>
     </row>
     <row r="392" spans="4:7" x14ac:dyDescent="0.2">
@@ -27185,7 +27190,7 @@
       </c>
       <c r="G480" s="2" t="str">
         <f t="shared" si="15"/>
-        <v>locations.dorm,</v>
+        <v>locations.dorm,//31 Choose your name Form</v>
       </c>
     </row>
     <row r="481" spans="4:7" x14ac:dyDescent="0.2">
@@ -28431,7 +28436,7 @@
       </c>
       <c r="G569" s="2" t="str">
         <f t="shared" si="17"/>
-        <v>-1,</v>
+        <v>-31,//31 Choose your name Form</v>
       </c>
     </row>
     <row r="570" spans="4:7" x14ac:dyDescent="0.2">
@@ -29677,7 +29682,7 @@
       </c>
       <c r="G658" s="2" t="str">
         <f t="shared" si="21"/>
-        <v>0,</v>
+        <v>0,//31 Choose your name Form</v>
       </c>
     </row>
     <row r="659" spans="4:7" x14ac:dyDescent="0.2">
@@ -30923,7 +30928,7 @@
       </c>
       <c r="G747" s="2" t="str">
         <f t="shared" si="23"/>
-        <v>-1,</v>
+        <v>-1,//31 Choose your name Form</v>
       </c>
     </row>
     <row r="748" spans="4:7" x14ac:dyDescent="0.2">
@@ -32169,7 +32174,7 @@
       </c>
       <c r="G836" s="2" t="str">
         <f t="shared" si="27"/>
-        <v>-1,</v>
+        <v>-1,//31 Choose your name Form</v>
       </c>
     </row>
     <row r="837" spans="4:7" x14ac:dyDescent="0.2">
@@ -33415,7 +33420,7 @@
       </c>
       <c r="G925" s="2" t="str">
         <f t="shared" si="29"/>
-        <v>-1,</v>
+        <v>-1,//31 Choose your name Form</v>
       </c>
     </row>
     <row r="926" spans="4:7" x14ac:dyDescent="0.2">
@@ -34661,7 +34666,7 @@
       </c>
       <c r="G1014" s="2" t="str">
         <f t="shared" si="31"/>
-        <v>-1,</v>
+        <v>-1,//31 Choose your name Form</v>
       </c>
     </row>
     <row r="1015" spans="4:7" x14ac:dyDescent="0.2">
@@ -35907,7 +35912,7 @@
       </c>
       <c r="G1103" s="2" t="str">
         <f t="shared" si="35"/>
-        <v>-1,</v>
+        <v>-1,//31 Choose your name Form</v>
       </c>
     </row>
     <row r="1104" spans="4:7" x14ac:dyDescent="0.2">
@@ -37153,7 +37158,7 @@
       </c>
       <c r="G1192" s="2" t="str">
         <f t="shared" si="37"/>
-        <v>"null",</v>
+        <v>"null",//31 Choose your name Form</v>
       </c>
     </row>
     <row r="1193" spans="4:7" x14ac:dyDescent="0.2">
@@ -38399,7 +38404,7 @@
       </c>
       <c r="G1281" s="2" t="str">
         <f t="shared" si="39"/>
-        <v>"null",</v>
+        <v>"null",//31 Choose your name Form</v>
       </c>
     </row>
     <row r="1282" spans="4:7" x14ac:dyDescent="0.2">
@@ -39645,7 +39650,7 @@
       </c>
       <c r="G1370" s="2" t="str">
         <f t="shared" si="43"/>
-        <v>"null",</v>
+        <v>"null",//31 Choose your name Form</v>
       </c>
     </row>
     <row r="1371" spans="4:7" x14ac:dyDescent="0.2">
@@ -40891,7 +40896,7 @@
       </c>
       <c r="G1459" s="2" t="str">
         <f t="shared" si="45"/>
-        <v>0,</v>
+        <v>0,//31 Choose your name Form</v>
       </c>
     </row>
     <row r="1460" spans="4:7" x14ac:dyDescent="0.2">
@@ -42137,7 +42142,7 @@
       </c>
       <c r="G1548" s="2" t="str">
         <f t="shared" si="49"/>
-        <v>false,</v>
+        <v>false,//31 Choose your name Form</v>
       </c>
     </row>
     <row r="1549" spans="4:7" x14ac:dyDescent="0.2">
@@ -43383,7 +43388,7 @@
       </c>
       <c r="G1637" s="2" t="str">
         <f t="shared" si="51"/>
-        <v>-1,</v>
+        <v>-1,//31 Choose your name Form</v>
       </c>
     </row>
     <row r="1638" spans="4:7" x14ac:dyDescent="0.2">
@@ -44629,7 +44634,7 @@
       </c>
       <c r="G1726" s="2" t="str">
         <f t="shared" si="53"/>
-        <v>-1,</v>
+        <v>-1,//31 Choose your name Form</v>
       </c>
     </row>
     <row r="1727" spans="4:7" x14ac:dyDescent="0.2">

</xml_diff>